<commit_message>
[Expression] - [NUMBER >> roundTo]: custom decimal rounding support via [`nexial.number.rounding`]
[number]
- [`roundTo(var,closestDigit)`]: custom decimal rounding support via [`nexial.number.rounding`]

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_numberCommand.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_numberCommand.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB000AE-DDE2-2747-BF84-1D626D23FF11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A34CE61-418C-4F7D-B564-C113D54914E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="-4360" windowWidth="38400" windowHeight="10580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>true</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>nexial.scope.iteration</t>
+  </si>
+  <si>
+    <t>nexial.delayBetweenStepsMs</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -510,15 +516,15 @@
   <dimension ref="A1:AAA4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.1640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="1" max="1" width="31.375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
@@ -542,6 +548,12 @@
       <c r="AAA2" s="4"/>
     </row>
     <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="HA3" s="5"/>
       <c r="AAA3" s="6"/>
     </row>

</xml_diff>